<commit_message>
Get daily reddit data: Tue Dec 17 08:12:03 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_22.xlsx
+++ b/data/collected_data/2024_12_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C498"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,3355 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1hg5pmm</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Builder Gel Infill Question</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hg5pmm/builder_gel_infill_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1hg5hhq</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>I missed hiving long nails so bad 😔🫶🏻</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg5hhq</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1hg5d83</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>🩷did these divalicious nails 💚</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7jbcusna1d7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1hg53y4</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Christmas Ornament Nails 🎄</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg53y4</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1hg51c9</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>Christmas and New year's nails in one set 😍 in loveee with how they tuned out (glitter is sometimes a hit or miss)</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg51c9</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1hg4x7k</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>my last two sets 💅🏾✨</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg4x7k</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1hg4nbu</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel x help </t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg4nbu</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1hg4jjl</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you tip nail techs if they make their own prices? </t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hg4jjl/do_you_tip_nail_techs_if_they_make_their_own/</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1hg4gk4</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Winter nails🤍</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg4gk4</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1hg44h1</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>My turn ❄️🎄✨️</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg44h1</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1hg3gzn</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HELP - What is a nail polish color that I can buy in the US closest to this color?? </t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg3gzn</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1hg3gg2</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>Fresh mani</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q27qdqzjec7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1hg32ce</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Went simple this year. I wish there was more sparkle 😩</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjwv9tziac7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1hg2jrj</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>how to fix/care for nail filed down too far</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg2jrj</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1hg2vsl</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>🖤⭐️🤍</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg2vsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1hg2u1s</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ho Ho Ho </t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg2u1s</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1hg2rwc</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Matte Black French tip with little bow detail 🖤</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg2rwc</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1hg2dx0</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Newest nails</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kz0kzt5d3c7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1hg24y1</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>My Christmas mani</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg24y1</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1hg1xms</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg1xms</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1hg0spu</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These nails are super beautiful </t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w0ra7l60ob7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1hg1rhf</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Ending my day, I hope you like my work. 🙏🏻🥰</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxypcq08xb7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1hg0hzd</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>How to get hard gel off at home</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hg0hzd/how_to_get_hard_gel_off_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1hg05k6</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>LoZ inspired nails for my bday</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg05k6</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1hg1p37</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dip powder much darker than swatch </t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg1p37</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1hg1gra</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Everyone had something to say about my nail length back when I wore them like this (I also did a shorter almond sometimes) but it’s been almost 3 years since I had disposable income to maintain them and I still have phantom nail extension sensations. This is OPI Nessie Plays Hide &amp; Sea-k. </t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcx3hkp9ub7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1hg14rn</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>Does anyone have the sizes in mm for these nails?</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2u51gsi4rb7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1hg0ty5</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Violet Floral</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kbrxr4bob7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1hg0m7a</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Jinx nails!</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg0m7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1hg0l4h</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>new set</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v2pnyapylb7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1hg08xs</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Winter nails ❄️</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg08xs</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1hg04yx</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>the melting snowman trend is my fav this year 🥹</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z9eo72uohb7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1hfzyw0</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New stunningly beautiful gel winter wonderland snowflake nails! </t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r9erhlw5gb7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1hfzs80</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My pink and purple Christmas nails </t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfzs80</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1hfzr65</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My 15 year old set up a table in my living room </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amoe3kz7eb7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1hfzgal</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Showing today’s Holiday ‘Cat Eye’ Gel Nails!</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mm2ggmbebb7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1hfz3si</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>Might be a dumb question but..</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qnu8br98b7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1hfz25o</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Winter wonderland</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfz25o</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1hfybqg</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Festive nails</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfybqg</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1hfxka9</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any advice on how to my nails more almond shape? They look kinda of wonky to me </t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qpmyue73va7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1hfx8hq</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Wintery Night Nails</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfx8hq</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1hfwued</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>"The Santa Clause" (left) &amp; "Home Alone 2" (right) themed nails</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfwued</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1hfwqb3</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Christmas ready ! </t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d28v76p6oa7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1hfwhob</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>3D Fuzzy Paw Nails 💕🐾</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfwhob</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1hfw9wo</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Christmas/team spirit Nails</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5fzbcggka7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1hfv6fk</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>I present to you a design I made inspired by my daughter, what do you think? I have it saved as a memory</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uuz1swysba7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1hfvu11</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>Green with envy? 💚💚</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sthqnpdtga7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1hfvso9</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Christmas nails done by me ❤️🎄🐈‍⬛️💚</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfvso9</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1hfvkhx</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Question for those who know how to or are able to do it. If for my hand it will fit round or square nails?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sc3mglhwea7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1hfvh3g</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>Psychogenie figure twin</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfvh3g</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1hfuivv</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>A beautiful design for my queen.</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0lt5ab3w6a7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1hfsxpm</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my own Christmas nails </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfsxpm</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1hfsgm4</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Graduation nails</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfsgm4</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1hfscqm</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>First Post here 🎀😇</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kdekrh1eq97e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1hfsbw0</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love these so much! </t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfsbw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1hfs8zb</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Lilac chrome</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfs8zb</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1hfs3gt</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>I posted yesterday before I went to get a fresh manicure. These are my current nails. I love them .</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfs3gt</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1hfrplf</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Vacay Acrylics!!</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfrplf</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1hfrofh</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Hope you like them. ❄️🎄🎁🌲</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlfhnccel97e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1hfrgvi</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my holiday nails🥹 did them myself!! </t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfrgvi</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1hfr3te</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>I like my new French manicure</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lvcy8bczg97e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1hfr1dr</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfr1dr</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1hfqyej</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Gel Builder extensions possible on my nails?</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n0t6z3qzf97e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1hfqmur</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>Least damaging nail extensions</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hfqmur/least_damaging_nail_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1hfqngh</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thought they were cute at first but someone said they look like the poop emoji and I can’t unsee it now </t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cm19we3qd97e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1hfq2e4</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Christmas nails ❤️💛</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zct0u77g997e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1hfpqxk</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">help please </t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfpqxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1hfowig</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pearl chrome application error? More opaque than expected </t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfowig</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1hfpatr</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Deer/fawn set I did!</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfpatr</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1hfoz9l</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>In love with this design</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yfud37ud197e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1hfov65</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Should I go back?</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tnv2hnsj097e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1hfokb5</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Icy nails ❄️</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzufqe1by87e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1hfhmzv</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>What do I need?</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hfhmzv/what_do_i_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1hfkrn6</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>I made these nails for 3 hours🤪 what do you think?</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2sei8bcn487e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1hflb15</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Does this mean my nail is about to break??</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hflb15</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1hfgu7a</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Bubbling in press-ons after applying adhesive remover?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfgu7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1hfea9g</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>just finished doing my Christmas set!! what do you guys think?</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfea9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1hfj1oa</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using builder gel! </t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2gudviqp77e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1hfmt3i</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas 💅 </t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x918bgixk87e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1hfnnu8</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Nails chipping after 2 days</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfnnu8</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1hfnnb9</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Dazzle dry</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8fha3kgr87e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1hfn68t</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>Finished Painting My Nail Set for Christmas 🎁</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfn68t</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1hfn4ff</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help getting engagement nails today! </t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfn4ff</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1hfmx0v</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Merry Christmas 🎄 </t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfmx0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1hfms77</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Wasn't sure I wanted to post these, since I want to retry this technique... thoughts on how I can do it better?</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fhml9nypk87e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1hfmrg6</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Holiday Nails</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fazte0lkk87e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1hfmnww</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>so proud of this set❤️</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfmnww</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1hflugh</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Chamaeleon Nails - Desert Bandits 🌵👽</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hflugh</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1hfktrm</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Sparkly nails for Christmas: because nothing says holiday cheer like a little glitz!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://v3.redgifs.com/watch/incompatibleunlinedblueandgoldmackaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1hfks8s</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>gel nails on myself!</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfks8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1hfkkk7</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Help with Semi-Permanent Manicure: Polish Spreading</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hfkkk7/help_with_semipermanent_manicure_polish_spreading/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1hfkgv1</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>My Christmas nails as somebody that loves grey and black tones</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zp5ead5287e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1hfjx4r</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>glitter and chromo nails😌</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/biq0arshx77e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1hfjvte</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple green nails </t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v68o9cg5x77e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1hfjusb</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what do we think about this set </t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ru9feo9ww77e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1hfjte7</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>did my friends nails today</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nas0z3jjw77e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1hfjqzo</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>I love this set</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hj4dz7czv77e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1hfjpwc</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Red nails😊</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8vak3qrv77e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1hfjk9p</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>When you find an awesome nail tech, never let them go!</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfjk9p</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1hfj79p</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Starting out the cold winter season with holiday nails to keep me in good cheer. </t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l9dqrteuq77e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1hg5hup</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Sassy sauce Absinthe Minded and Twisted Terracotta Tanzanite thermal shift</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg5hup</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1hg444j</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Trying out first polish from an indie creator</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49fnkxwxlc7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1hg3r8q</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Winter Mani</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg3r8q</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1hg3aem</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Finally caved and bought a Moon Cat polish</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7e9shzurcc7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1hg2x6t</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Got my LynBDesigns BF order today!</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qg029kny8c7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1hg2p3w</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>The way the ILNP bottles fit together. 😌</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ty5kh8pk6c7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1hfpa8t</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>Beetlejuice, beetlejuice, beetlejuice by Vanessa Molina</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfpa8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1hfnngb</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Absolutely in love with my current nails 💫</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfnngb</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1hfjb4o</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Nails Inc. thermal in the shade “Degree In Hot” ⭐️</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l71vc6n4s77e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1hg28o4</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>The Great Cuticle Oil Debate</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hg28o4/the_great_cuticle_oil_debate/</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1hg27ch</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Glowiest Glow in all the Land?</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hg27ch/glowiest_glow_in_all_the_land/</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1hg25mb</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Input needed: Color sorting</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6hkgfq31c7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1hg1yw8</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Festive mooncat BF haul!</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg1yw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1hg1xpo</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>trying a new indie brand + GWP!</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg1xpo</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1hg11q9</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>All the greens</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2jqjo9hcqb7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1hg0svi</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mood Ring </t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg0svi</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1hg0d6t</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Mooncat Poisonberry</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg0d6t</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1hg0889</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Bluebird Lacquer, ❄️Winter Is So Chill❄️</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f05s02yjib7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1hfzmuu</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Lurid Love</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfzmuu</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1hfzm2d</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>Feeling springy and greeny! 🐸 🌱</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfzm2d</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1hfzkzl</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Christmas lights!!!!</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfzkzl</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1hfzdyh</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Attempt at nail art on my natural nails</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ha7g1scsab7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1hfz1w0</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>Holo Taco Topper</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hfz1w0/holo_taco_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1hfxtvb</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>My bestie gave me a Christmas themed manicure 🎄</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfxtvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1hfxn4y</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Okay, I did it! I bought the Bisley. </t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y4a9bz0sva7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1hfxmdt</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Colors that don’t flatter your skin tone?</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hfxmdt/colors_that_dont_flatter_your_skin_tone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1hfxh4e</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>What is the prugliest polish you have ever seen/bought/worn?</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hfxh4e/what_is_the_prugliest_polish_you_have_ever/</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1hfx6m7</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Indie options for good creme colors? </t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7qygbau0sa7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1hfx5eb</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Something festive! 🎄🎀✨</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfx5eb</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1hfwy3n</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>can’t decide if i like these or not!</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfwy3n</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1hfwaf6</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Your Heart's a Black Hole</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bxw0y7flka7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1hfvkad</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>I never got HT Frozen Benanas, but I think I made a pretty good approximation of it</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfvkad</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1hfvc10</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Fancy Gloss has fulfilled my thermal dreams!</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfvc10</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1hfu4t6</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>Salvaging a polish that doesn't work for you?</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/247k3tty3a7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1hftx3q</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Small case recommendation?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hftx3q/small_case_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1hftv1o</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>My first (and modest) Lurid Lacquers Haul!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hftv1o</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1hft2sv</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Skye in the sky </t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hft2sv</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1hfskly</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Atomic “Prototype” - who is she </t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfskly</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1hfs42w</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Similar glitter toppers to OPI's I Snow You Love Me?</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hfs42w/similar_glitter_toppers_to_opis_i_snow_you_love_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1hfs396</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>OPI Let's get scrooged</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfs396</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1hfrts7</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Show me your Christmas manis! I'm enjoying these festive tips right now</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6t4kr8ekm97e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1hfr9pl</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Does this count as a holiday green? 🤭</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfr9pl</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1hfqoym</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>FOMO buying— new to indie polish &amp; need tips</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hfqoym/fomo_buying_new_to_indie_polish_need_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1hfql2g</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holy hell, my first Sassy Sauce polish did not disappoint! </t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfql2g</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1hfqh9o</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>Please help me save her</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2q6bn2jc97e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1hfqh2p</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Christmas mode: activated</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0jfesurhc97e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1hfq8rw</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>It's beginning to look at lot like Christmas!</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vqubv3m6a97e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1hfq736</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>getting in the holiday spirit 🎄🎁✨</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfq736</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1hfq5cy</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Blue Christmas 😘</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g0exdzl2a97e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1hfq2v4</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t xml:space="preserve">✨💡Let it glowww (part 2) Outdoor lighting </t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfq2v4</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1hfpuf9</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Magnetic nails + Stamp!</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfpuf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1hfpkyu</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Oh Look it’s Scowly Face 🤭</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfpkyu</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1hfpiel</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>All the Feelings 2.0- Emily de Molly</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hfpiel/all_the_feelings_20_emily_de_molly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1hfpgnw</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>✨️💚Holly Jolly💚✨️</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfpgnw</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1hfpf5r</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fashion Polly! </t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfpf5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1hfo8eo</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First Sassy Sauce order was a success.  Pictured: Subterfuge, a hot pink with a copper penny shift in extreme angles. </t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfo8eo</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1hfo7e9</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Feel like a Midwest princess</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfo7e9</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1hfnzm4</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Serpents of Eden  Color Review</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfnzm4</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1hfnwrh</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Gran loved her butterfly nail combo 🦋✨️</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfnwrh</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1hfntaq</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Extra sparkly to cope with the shorty chop!</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bs4w2nr9s87e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1hfn4ge</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Snowy Glowy Skittle</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfn4ge</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1hfmrsd</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>Guidance for a beginner</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hfmrsd/guidance_for_a_beginner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1hfmo41</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails Brittle and Peeling After New Mooncat Mani? </t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hfmo41/nails_brittle_and_peeling_after_new_mooncat_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1hfltbl</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Chamaeleon Nails - Desert Bandits 🌵👽</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfltbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1hfltao</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first attempt at gel polish! </t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfltao</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1hflg6l</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t xml:space="preserve">deep space for my birthday nails this week! 🥳 </t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hflg6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1hfl9ur</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>Trying out a new nail shape❄️</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfl9ur</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1hfkimg</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Simple pale pinks on natural nails ft our Xmas decorations💗</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfkimg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1hfke4n</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Can someone eli5 gel manicures to me?</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hfke4n/can_someone_eli5_gel_manicures_to_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1hfjoip</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice for a two week trip? </t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hfjoip/advice_for_a_two_week_trip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1hfih9k</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>So /Tired/ of researching ‘HEMA free’ brands, pls help</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hfih9k/so_tired_of_researching_hema_free_brands_pls_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1hfh9yv</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>It's me , back again with glitters 🤌🏻😭🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfh9yv</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1hfgp69</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hfgp69/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1hffao1</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Which nail shape for wide bed nails?</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hffao1</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1hfeyqm</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>A cute rainbow jelly skittle mani 🌈</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aoemg78dc67e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1hfele9</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>Holy Grail base coat suggestions pls - from a Canadian!</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hfele9/holy_grail_base_coat_suggestions_pls_from_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1hfeisg</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Witchcult Mistletoe + Nail Art &amp; Stickers</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfeisg</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1hg5eef</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Divalicious nails I did </t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bz9xyc9q1d7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1hg50aq</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Sweetie Pie Set</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg50aq</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1hg3e0u</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>A Christmas Story</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg3e0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1hg2620</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Starry Night Set</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ga3jfpq71c7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1hg226n</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of my works! Merry Christmas 🎄 </t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v6ya86j50c7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1hg0oyz</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Jinx nails!</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg0oyz</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1hfysj9</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>#HoodNails</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfysj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1hfyh41</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unintentionally made some Wicked nails😂 </t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ki15ft4v2b7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1hfybq5</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Punk Nails </t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9q1hvk4m1b7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1hfy31n</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beautiful </t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t3za5wljza7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1hfxvpw</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gingerbread nails 💅🏻 ❄️ </t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfxvpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1hfpwqm</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Winter nails ❄️</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfpwqm</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1hfommm</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Where are those who love blue?</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfommm</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1hfn5x4</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Finished Painting My Nail Set for Christmas 🎁</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hcbpbfon87e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1hfm526</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>Best matte GEL topcoat?</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hfm526/best_matte_gel_topcoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1hfl2nn</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Holiday Set</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lnip7a3787e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1hfl01l</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginner needing confidence </t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hfl01l</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1hfkaxt</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>beautiful design for christmas. do you like it?</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l36o1l9r087e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1hfihjo</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Red for Christmas time! Do you like it?</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xw3v0a3dk77e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1hfhpzs</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Christmas hand painted nails! ❄️</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4peedf72c77e1.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Dec 18 08:11:42 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_22.xlsx
+++ b/data/collected_data/2024_12_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C498"/>
+  <dimension ref="A1:C675"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8899,6 +8899,3015 @@
         </is>
       </c>
     </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1hgwxde</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Fresh</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgwxde</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1hgw37d</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>Pain like hell during UV light</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgw37d/pain_like_hell_during_uv_light/</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1hgv7kw</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>I’m trying press on half tips with regular polish but I know I need to buff. Would a buffer make the nail flesh with the skin, because I don’t want to use a drill on my nails?!</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgv7kw</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1hgvpvy</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Question On What/How To Ask A Tech For This…</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgvpvy/question_on_whathow_to_ask_a_tech_for_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1hgvq6j</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>NEW COLOR 🤩🤩🤩</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgvq6j</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1hgvhax</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Been on a fruit-nail kick lately 🍓 </t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgvhax</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1hguwaf</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>New nails 💕 I know it's the holidays but...</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42sme00xnj7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1hguf5s</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Birthday nails 💅🏼</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fyfiyrogij7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1hgtjtu</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glow in the Dark Nails! </t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hjywdbyd9j7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1hgt83d</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Design </t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lj2cf6d86j7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1hgsp5h</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Why do my thumb press ons pop off so quickly compared to the rest of my fingers?</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgsp5h/why_do_my_thumb_press_ons_pop_off_so_quickly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1hgsvhq</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t xml:space="preserve">help with builder gel routine please! </t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgsvhq/help_with_builder_gel_routine_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1hgsthm</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Birthday set ♑️</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgsthm</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1hgsp2f</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Christmas set!</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9u49312x0j7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1hgs995</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>We like to match 💅</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgs995</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1hgrzb1</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple Christmas nails </t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/paope4ozti7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1hgrk7i</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>First Nail Art Attempt!!</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uu098fuxpi7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1hgrg37</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Got my Winter nails done today! </t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgrg37</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1hgrcid</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>First time using cat eye gel</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/awerav9wni7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1hgr21h</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>my cousin made my press-ons 💚</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgr21h</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1hgq09f</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t xml:space="preserve">some of my fav nails from the last few months </t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgq09f</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1hgqmbb</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does the almond nail shape suit me? </t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgqmbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1hgqg1w</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>back to gel manicures</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lgffnpnkfi7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1hgqbvm</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>christmas nails!</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2a33ak7iei7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1hgpplp</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>An extra from my best friend that I made 3 days ago 💖</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x60nowgu8i7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1hgpn4x</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>With these 2 designs made with a lot of love I close my work day 😘😘😘</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgpn4x</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1hgpj84</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>holiday nails done on myself, gel-x</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/upufnsfc7i7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1hgparo</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t xml:space="preserve">If I use regular nail polish and paint over it with gel top coat, will it last as long as gel? </t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgparo/if_i_use_regular_nail_polish_and_paint_over_it/</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1hgoyz5</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>New favorite set!</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgoyz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1hgowwz</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>First Time Doing Gel Nails – Tips and Feedback Wanted!</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgowwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1hgorqt</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Nail tech filed down into my nail bed? Will this heal as my nail grows or is it permanently messed up?</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgorqt</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1hgnxjh</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Which ones should I wear Xmas day? 👀 I’m torn!</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1q4tyrlcth7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1hgoosj</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>I nails express tip</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgoosj/i_nails_express_tip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1hgnvnb</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Best winter color for nails???</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgnvnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1hgnuu4</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Another set my talented sista did for me:) </t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgnuu4</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1hgnrm3</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>My sister did these for me :)</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7wimik1zrh7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1hgnnti</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink definitely says Christmas, right? </t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2ecqvy4rh7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1hgmzn8</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Is this normal? Done in a professional salon, paid €45. First time getting them painted so not sure if I’m right to complain.</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgmzn8</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1hgmltd</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>First time getting nails like this!</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7hm1swklih7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1hgmcp6</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>Does this colour suit me</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbj009qlgh7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1hgm647</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Gelx removal - builder gel</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgm647/gelx_removal_builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1hgm050</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>Christmas nails❤️✨</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fkli1ynvdh7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1hglkqq</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>I told my nail tech I wanted the glitteriest nails she’s ever seen and I think she delivered… ✨</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43z4lorjah7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1hglhii</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hglhii</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1hglew1</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>christmas mani 😩</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hglew1</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1hgl8k0</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Can you guys make me feel better?</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgl8k0</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1hgl77i</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Don't be like me.</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgl77i</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1hgktbk</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>Dansko inspired Blue chrome- icicles!❄️🥶</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgktbk</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1hgkmjq</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>The color of the season</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgkmjq</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1hgkvy6</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Purple 💜💜</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6fotfo245h7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1hgki2w</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Anyone feel like gel x makes their natural nails flat?</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgki2w/anyone_feel_like_gel_x_makes_their_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1hgk4sd</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>gingerbread nails</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0b1mixwyg7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1hgk403</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t xml:space="preserve">peppermint cat eye set for christmas 🌟 </t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgk403</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1hgjxg3</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Favorite set</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgjxg3</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1hgjver</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>basic gold n white christmas/nye set ૮₍ ˃ ⤙ ˂ ₎ა</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgjver</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1hgjlqn</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t xml:space="preserve">beetles nail polish </t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgjlqn/beetles_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1hgjh2c</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>I guess you could say I was a little inspired by the color scheme of Arcane &amp; Jinx art 💥</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgjh2c</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1hgjg3z</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>honest opinion guys and gyals ?</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ylcschhctg7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1hgjbaw</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Absolutely love a cat eye manicure</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgjbaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1hgjako</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Hypothetical situation for anyone who does nails (professionally or hobbiest): Say your favorite client who has been going to you for years is an old lady. Yesterday, she peacefully passed away in her sleep. Her family is requesting, on her behalf, that you do her nails one last time. Would you?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgjako/hypothetical_situation_for_anyone_who_does_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1hgizma</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>Christmas Set! (don’t mind the scratches… I learned my new drill bits are good the hard way 🫡)</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ehm5i6ypg7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1hgiy4v</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Chamaeleon Nails - Senua</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgiy4v</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1hgix86</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My winter Christmas nails! </t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rt2mlfwfpg7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1hgix3i</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Any advice on a electric nail file for kids?</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgix3i/any_advice_on_a_electric_nail_file_for_kids/</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1hgiwl8</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Im a beginner nail tech who’s practicing nails in my bedroom, how can I do nails in my room and minimize the monomer smell? </t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgiwl8/im_a_beginner_nail_tech_whos_practicing_nails_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1hgiwi8</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>no chip top coat = more chipping?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgiwi8</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1hgir60</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Feeling frosty with my new nails 🥶🩵</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgir60</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1hgillb</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>My Christmas Nails 🎄</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfwnfiqwmg7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1hgicnx</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>My latest after a fill in.</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wu7qzm9ykg7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1hgic41</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>New Christmas nails</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgic41</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1hgi5jz</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Help Choosing a Safe Option</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgi5jz/help_choosing_a_safe_option/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1hgi88a</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>DIY original designs</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgi88a</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1hgi1wv</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Fashion avenue - Barbie serie season 1</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgi1wv</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1hghy60</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Two weeks ago I posted about my nails</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hghy60/two_weeks_ago_i_posted_about_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1hght2x</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Some glitter for the holidays ✨ What do you think?</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jok8c8osgg7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1hghs5l</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>My favourite time of the year🎄 New set for my friend</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hghs5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1hghou3</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>I tried to do tortoise print, but at a red one</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8d6qbddufg7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1hghl0a</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Festive enough?</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hghl0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1hghjc9</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>🍫🤎</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i7wktcrqeg7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1hghgxw</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>101 Dalmatians nails 🐾</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hghgxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1hghabk</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>🩷❄️✨</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hghabk</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1hghaup</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Christmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/141klafwcg7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1hggy3v</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Im unstoppable </t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3rxmma48ag7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1hggvbc</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hello, I’m launching a web agency specifically for nail technicians. I will design and publish your website within 48 hours. What pricing do you think would be attractive for this service? </t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hggvbc/hello_im_launching_a_web_agency_specifically_for/</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1hggnvv</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>My girlfriend really likes doing her nails, is there anything you would never buy for yourself but would be really nice to have?</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hggnvv/my_girlfriend_really_likes_doing_her_nails_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1hggkvf</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Impressed myself with this gel x set</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hggkvf</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1hggev6</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Christmas set✨</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0hfnw3l56g7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1hgg4u7</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>I leave you 2 of my new designs made with a lot of love ❤️❤️🙏🏻</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgg4u7</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1hge3ih</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Strong and beautiful </t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hge3ih</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1hgg0f5</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Christmas set</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgg0f5</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1hgfdzy</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Nails = ruined</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgfdzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1hgfayr</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Is it hard to function? Yes. Do I still love them? Also yes 😭</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l347fwdpxf7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1hgeo7x</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Nail care after semipermanent manicure?</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgeo7x/nail_care_after_semipermanent_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1hgewki</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to make glitter stay on acrylic nails? </t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgewki/how_to_make_glitter_stay_on_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1hgeurq</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>Any recs for a really good strengthener?</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hgeurq/any_recs_for_a_really_good_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1hgekiy</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>Green and bronze Xmas nails</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgekiy</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1hgej4e</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Holiday Nails 🎁</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgej4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1hgedry</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>RIP to my natural nails at their peel perfection. Growing them back out after a few breaks. 🪦🥲</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gtj0dnepqf7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1hge4we</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Little gold set</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/80zz7k1rof7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1hge4j3</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Lookin like those candies old ladies always have in their purse 🍓✨</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hge4j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1hgw9s2</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t xml:space="preserve">looking for a  cuticle oil! </t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hgw9s2/looking_for_a_cuticle_oil/</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1hgviys</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>best dark brown? mooncat or DVN?</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hgviys/best_dark_brown_mooncat_or_dvn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1hguyqj</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>🪻dainty flowers 🪻</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hguyqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1hgu797</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>I can’t stop looking at them but I already want to change them 😅</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pvrvx0t4gj7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1hgsrqj</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What's that one product that surprised you. </t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hgsrqj/whats_that_one_product_that_surprised_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1hgsokh</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>Is Sinful Colors gone for good?</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgsokh</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1hgsem3</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>Indies that have a thicker non sheer formula?</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hgsem3/indies_that_have_a_thicker_non_sheer_formula/</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1hgr0le</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>Festive but make it soft summer</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/goaxgd4uki7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1hgq85c</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Swatch request:  Atomic’s Rum Ham vs. Mooncat’s Merkitten</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hgq85c/swatch_request_atomics_rum_ham_vs_mooncats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1hgpvwh</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>What can I use in replacement of a nail magnet?</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hgpvwh/what_can_i_use_in_replacement_of_a_nail_magnet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1hgpoh4</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>First Emily de Molly order, mini haul 🤗</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgpoh4</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1hgpnic</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>I’m loving this color combo</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4rr5r06g8i7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1hgpl0k</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t xml:space="preserve">To the nines! </t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgpl0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1hgojsq</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Mirror Ball vs Coconut Crush by Lakur</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0isf23aqyh7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1hgodo3</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone else still waiting on their Zoya BF order? </t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hgodo3/anyone_else_still_waiting_on_their_zoya_bf_order/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1hgo3rl</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t xml:space="preserve">polish saved my fingers! </t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgo3rl</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1hgntlm</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Merry Christmas from my mama</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgntlm</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1hgn1u8</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>CND Shellac Gel Polish - Emerald Lights</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oogqj9q4mh7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1hglzm1</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>first ombre! Any tips for sponge application?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hglzm1</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1hglq55</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Bee’s Knees Lacquer - She Was Enough</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hglq55</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1hglk7c</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Let’s Be Friends Forever-OPI</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72hrdkgfah7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1hglgel</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>ILNP Poison + Eclipse</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hglgel</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1hglaik</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>Christmas ready ❄️</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tuocj6gb8h7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1hgl138</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>One Coat Black by Holo Taco topped with Chemical X by Mooncat</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pr53vdu76h7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1hgkz4k</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Dazzle Dry in the UK?</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hgkz4k/dazzle_dry_in_the_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1hgkpov</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>How long did it take to “perfect” your painting technique?</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hgkpov/how_long_did_it_take_to_perfect_your_painting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1hgk2ao</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>Today’s mani</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jjb08mxbyg7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1hgjjda</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Cloudburst by Polished for Days</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgjjda</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1hgjbwb</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>Help!!!! Food dye has stained my nails😢😭</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n5kavm5lsg7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1hgj59w</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Maelstrom makes me really feel like a siren</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l5quzlk4rg7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1hgize9</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Chamaeleon Nails - Senua</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgize9</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1hgigv9</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>I’ve joined the Maelstrom fan club!</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgigv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1hgigui</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Year of the Ox by Dany Vianna</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8gfstqulg7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1hgidd3</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Looking for Help: Split nail bed?</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1x9hxu53lg7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1hgibjn</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>My first *kinda* successful attempt</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgibjn</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1hgi8n8</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Interstellar (movie inspo)</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ss1xif83kg7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1hgi3zu</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>Esmalte em gel</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yixlkkf3jg7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1hgi2tp</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>When a polish is even better than the swatch photos 😍</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vgzqy0lsig7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1hghaw4</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>kbshimmer's Kringle All The Way is super over the top and I love it.</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hghaw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1hgguk6</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>It’s a marshmallow world 🎶</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5oektx1h9g7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1hgggc4</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>✨Mystical shorties✨</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgggc4</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1hggd12</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Gingerbread nails with ILNP Prancer and Shapeshifter</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hggd12</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1hgftg5</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Gel removal ruined my natural nails</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8if13wk1g7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1hgey36</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blade of the Frontiers is sooo glassy! </t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/u4ssigl2vf7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1hfrnbc</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>Indie Brand Order Turn-Around Time Question</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hfrnbc/indie_brand_order_turnaround_time_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1hfsqeu</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Need help with a gift!</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>/r/lacqueristas/comments/1hfsoc2/need_help_with_a_gift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1hgdz0i</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t xml:space="preserve">For people who use swatch wheels: do you clean them or are they one-use for you? </t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgdz0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1hgd4sj</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>3 coats of Paloma by Zoya</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hte3v0brgf7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1hgcd4p</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Phoenix Indie’s Bill part 2</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xn3kpfaeaf7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1hgc9re</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Phoenix Indie’s Bill is so pretty under office lighting </t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgc9re</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1hgc55r</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>I'm such a sucker for such blackened polish with shimmer 😍</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qdbcgo1k8f7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1hgbqso</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>I just spent 3 hours trying to remove a salon manicure 😭</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hgbqso/i_just_spent_3_hours_trying_to_remove_a_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1hgba3w</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>Festive glittery green look using a Little Ondine shade!</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgba3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1hgars6</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Midnight Blue</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgars6</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1hgak0v</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Take No Shit. Do No Harm. </t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgak0v</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1hg9mx0</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Can I combine Neonail with normal nail polish?</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hg9mx0/can_i_combine_neonail_with_normal_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1hg9381</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Update on my damaged nails</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg9381</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1hg9225</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>I'm in Love ❤️</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg9225</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1hg8wlw</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>I feel like these need a sparkly topcoat or darker sheer on top, so that they match my skintone less!</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hue4cegrce7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1hg8jvs</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Any recs for a matte topcoat that actually stays matte?</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hg8jvs/any_recs_for_a_matte_topcoat_that_actually_stays/</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1hg89mu</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Holiday Nails</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vy5qf2pt4e7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1hg842f</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Swatchers on YouTube or Instagram with Asian (or Medium yellow undertone) skin tone? </t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hg842f/swatchers_on_youtube_or_instagram_with_asian_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1hg794e</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>ILNP - Flashing Lights</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg794e</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1hg6gt0</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Swatch sticks </t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hg6gt0/swatch_sticks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1hgwj80</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>I show you that today I made this design, and I loved it</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7l2vw4f18k7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1hgwfjm</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Black polka dots art</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgwfjm</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1hguikj</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Orchid set </t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bgfz79uhjj7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1hgrhw8</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>Cozy and cute this holiday season 🎄🎅🏻🤍</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3whz90ebpi7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1hgq7e9</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>I show you this work I did today! Encapsulated on soft gel!</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5zi2s2edi7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1hgi0am</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>Fashion avenue - Barbie serie season 1</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgi0am</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1hgee65</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set of acrylics In over a year of press ons </t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/opuiviasqf7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1hge71d</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Lookin like them candies old ladies always have in their purse.</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hge71d</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1hge5aa</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Little gold set </t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g30s8y7uof7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1hge341</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tiger set </t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ot64xgrcof7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1hgbk7e</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Clown nails</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kzriz8gh3f7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1hgam1j</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stained glass set </t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r8iktj0yue7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1hg8ok6</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Do you like it? I'm new to the world of nails. 💅</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hg8ok6</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Dec 19 08:11:23 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_22.xlsx
+++ b/data/collected_data/2024_12_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C675"/>
+  <dimension ref="A1:C872"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11908,6 +11908,3355 @@
         </is>
       </c>
     </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1hho75v</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Very cutesy </t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kgxl85h2kr7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1hhn2fe</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What service should I book for a teensy tiny bit of added length? </t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hhn2fe/what_service_should_i_book_for_a_teensy_tiny_bit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1hhmzre</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>Tropical holiday nails</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kc1xxqoq4r7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1hhmwi3</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>Press-Ons Feeling Tight - Take Off?</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hhmwi3/pressons_feeling_tight_take_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1hhluwu</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Shadow the hedgehog inspired nails by me!</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zhrwisvorq7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1hhm4w0</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>I was petting my dog and had to paws to snap a pic of the new nails</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/seh1c6nmuq7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1hhl8ps</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you size press on nails correctly </t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hhl8ps/how_do_you_size_press_on_nails_correctly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1hhk86v</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>Need Advice for glue on nails</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkj4edpmaq7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1hhkhui</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Hear me out.. This is not dirt</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/89as40gfdq7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1hhku3m</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Set </t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhku3m</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1hhk8de</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Holiday Engagement Nails</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhk8de</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1hhk39g</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>a beautiful gift and with this I end my great day at work 🙏🏻💙</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ig3fjy89q7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1hhjvu9</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>penultimate design today in the studio, I hope you like it 💍</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhjvu9</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1hhjnkx</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>My mami’s festive manicure ❤️</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rf4zyjfx4q7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1hhjj42</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Help! My nail art vs. inspo nail art from Pinterest by @Ilana Mayes / @glitterbels on insta</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhjj42</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1hhjix8</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Nail day-coquette blues</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3uc5oxrq3q7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1hhj5xy</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Question for the Nail techs out there, do you guys photoshop your clients hands before posting picture of your work?</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hhj5xy/question_for_the_nail_techs_out_there_do_you_guys/</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1hhiyb3</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>a little pink ✨🌸🩷</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhiyb3</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1hhj1di</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DIY Christmas Set </t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhj1di</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1hhivse</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>Holiday Frosty Nails 🥹❄️🥶</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnyrzbqnxp7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1hhgbng</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Help with gel nail polish</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hhgbng/help_with_gel_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1hhhi43</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t xml:space="preserve">options? </t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9irilrytkp7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1hhhd05</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Do you have to buff nails to get shellac/SNS etc. to adhere to it? </t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hhhd05/do_you_have_to_buff_nails_to_get_shellacsns_etc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1hhhaxb</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Chrsitmas nails ! </t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhhaxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1hhfqev</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>take me to the stars</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j5ap8d2d5p7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1hhf1xh</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>Made them today for myself😍</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhf1xh</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1hhexl9</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling Grinchy </t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2kxwizdiyo7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1hhex0c</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>help with ideal nail shape!</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhex0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1hherrz</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Green and glossy 😍</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qabgsc5xo7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1hherix</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>BLUE for Billie this weekend 💙💅🏼</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f8kb6872xo7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1hheov7</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Gel manicure won’t last</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hheov7/gel_manicure_wont_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1hhdw67</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can't decide if I love or hate them. Bonus doggies 🐕 </t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/js5pa5expo7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1hhef0r</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>White Christmas ❄️🤍</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhef0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1hhee98</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Nails </t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhee98</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1hhe7i2</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Do I have woman's nails? Wife saids so</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhe7i2</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1hhe049</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Super shorty holiday nails </t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhe049</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1hhdi1n</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Second time painting my nails</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ym10o23smo7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1hhdhz5</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love them 😍 </t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhdhz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1hhcwgh</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Christmas nails❤️ Share yours!</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhcwgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1hhcinn</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Back with another magnet gel set</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhcinn</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1hhbstg</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>My tech and I had so much fun on this set 💅🏻</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gaxi2cjj9o7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1hhbirv</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>🌸🌙🪻</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhbirv</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1hhb9nx</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Happy holidays! I love this Christmas Gel X set</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhb9nx</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1hhb6un</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Need help, idk what to do!</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hhb6un/need_help_idk_what_to_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1hhb0jn</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love my new nails </t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhb0jn</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1hhawdf</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>QUESTION! Gel polish wont cure on nail stand.</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hhawdf/question_gel_polish_wont_cure_on_nail_stand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1hhaqit</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>My first ever nails, any advice on how can I do better?</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhaqit</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1hhao44</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Birthday Gift</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hhao44/birthday_gift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1hh9uie</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>Winter set as a beginner</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh9uie</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1hh9jub</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails 💅 </t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh9jub</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1hh958h</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>First time doing gel nails. Please give me feedback if you have any 😊</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh958h</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1hh8uyn</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>christmas nails❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh8uyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1hh8reh</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday set </t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xiipsx69mn7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1hh8qv2</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Second attempt at Polygel</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh8qv2</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1hh82zt</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>All the Christmas/winter sets I've made (so far)</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh82zt</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1hh73ch</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried cat eye </t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh73ch</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1hh72hc</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Decided to try a different shape! Loving it!</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oiqw04899n7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1hh6v1n</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>I hope you like this design, I loved it. 🥺❤️</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh6v1n</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1hh6s9b</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Finally stopped biting</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh6s9b</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1hh5py2</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>Nail stickers</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hh5py2/nail_stickers/</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1hh5qa3</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>I want to match this color, any hints?</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7t0bqvqvym7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1hh5o9r</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help with long nails lasting </t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh5o9r</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1hh5mcn</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>My Christmas nails</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zydjra4ym7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1hh55f0</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Just a Trans Woman who loves Christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh55f0</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1hh3069</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Can I change the length / color of a Gel X manicure?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wjpf2shscm7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1hh25j4</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>Christmas Nails 🎄🎅🏼❤️</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh25j4</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1hh1bwl</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I overreacting? Ski slope nails. </t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh1bwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1hh1k0d</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best Nail Glue? </t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hh1k0d/best_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1hh4inb</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Nails </t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh4inb</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1hh48ir</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>White Christmas ❄️</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh48ir</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1hh45as</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>New month, new set</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh45as</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1hh438j</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>I got a soft gel mani exactly one week ago. Just took a shower, and the polish bubbled up everywhere. Why would this happen?</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yjxofdxxlm7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1hh3ecq</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>I'm inlove</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxyvvk46gm7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1hh2rgn</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Currently OBSESSED with my last set of the year</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh2rgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1hh2py5</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Rosa para la princesa 🎀</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2jiqid8am7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1hh1xer</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Snowflake nails</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1kgm47953m7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1hh13xa</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Christmas and New year nails</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ab9jwib8vl7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1hh0rv0</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>Another set of Christmas nails</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh0rv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1hh0obe</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Ready for Christmas!</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5z9rssuql7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1hh0gzc</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to take care of my nails. </t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh0gzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1hh0czu</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What nail shape do you think would look best on me? </t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2acisf4enl7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1hh0a6p</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>Timeless, elegant red nails for this Christmas ❤️🎄</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nrxatw6lml7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1hh089o</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>I broke my nail before my appointment</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh089o</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1hh032p</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>DIY festive nails!</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh032p</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1hgzwrw</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>First time doing press ons</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgzwrw</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1hgz8pc</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>🎄🎁</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jte3fdap9l7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1hgz8gl</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Starting the day I hope you like my design 💙</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgz8gl</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1hgz396</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>This is from mooncat and I love it</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aaa4swyq7l7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1hgywjq</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t xml:space="preserve">simple pink pearly jelly nails for xmas!! </t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzrlfrv85l7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1hgyqsy</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>New to getting my nails done and have questions about BIAB!</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3dkjvfc23l7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1hgxm8d</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Found a lil rainbow to take a picture of my new set🌈 Icy pink tips with jewels and charms❄️💕 </t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgxm8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1hho3f3</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>The first set I’m really proud of!</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qqdbdygpir7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1hhmuvp</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>engagement calls for a fresh at home mani :)</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/94bmhg713r7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1hhmuan</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>Don't sleep on Cupcake Nail polish!</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhmuan</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1hhlxhw</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My 3 month collection </t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhlxhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1hhls8q</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Polishes that look like this?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8ibue4awqq7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1hhlrj6</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>My nails may be super short but they're still cute!</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhlrj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1hhkhz4</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>Can I re-apply a “popped peely”?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hhkhz4/can_i_reapply_a_popped_peely/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1hhkhue</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t xml:space="preserve">lurid lacquer 😍 </t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhkhue</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1hhkgjq</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dupe for "Enemies to Lovers" by Lights Lacquer </t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rtv17kd1dq7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1hhkdcn</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Just a simple Christmas string lights inspired skittle</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/64jtmijwbq7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1hhk6o7</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>Why do I always sleep on mattes? 🌹</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhk6o7</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1hhjv87</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gave up on christmas nails, did jade nails instead ✨ </t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhjv87</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1hhjr4m</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>First post, Christmas nails</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhjr4m</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1hhjch6</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Where to buy By Vanessa Molina from Canada</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1boyya12q7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1hhj6l7</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>ilnp faun 😍</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0ilp5lih0q7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1hhinqb</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Got my Mooncat x Star Wars set</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhinqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1hhihuy</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>First Christmas colors of the season!</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mzrgr3sytp7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1hhifzy</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Grinch nails + peeling from cuticle remover?</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbzng5litp7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1hhi56m</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>So excited about my ilnp order</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhi56m</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1hhhttm</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can someone help me find the polish I'm thinking of? I used to adore it. It was matte, and I thought it was sally hensen but I can't find it.. It sorta had a creme color and bronze/gold flecks. Square bottle white lid. </t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hhhttm/can_someone_help_me_find_the_polish_im_thinking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1hhh0k7</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Winter jewel toned skittle</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhh0k7</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1hhh0f5</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Holiday nails that I feel so proud of! 🎄</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40c6m8icgp7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1hhgpx8</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Thank you for influencing me, this polish is UNREAL!</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y2f7otosdp7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1hhgcr8</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Green Eyed Monster is so fun for winter</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xy3i4mlkap7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1hhfzka</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>Interstellar Nails 🌌</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/767tqgdg7p7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1hhfevj</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some new faves from Mooncat </t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhfevj</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1hhf9vu</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Tried a skittle for the first time and got the perfect birthday nails! 🥳</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhf9vu</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1hhf5xf</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Green with gold flake topper</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhf5xf</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1hhf1si</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>Does anyone know of a dupe for the hot pink shade in KBShimmers Aft Backwards?</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tucgeyg6zo7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1hhey32</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>River Styx really is that girl ✨</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zkb1pekmyo7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1hhetyb</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Velvet and straight line</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhetyb</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1hheqhn</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Oops, didn’t realize</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ipsgc8quwo7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1hhei0e</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t xml:space="preserve">One of my students said my nails look like cookie icing ❄️ </t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhei0e</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1hhecpe</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Moody Christmas mani</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/23es1efqto7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1hhds3w</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>First time doing my nails in a long time</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhds3w</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1hhdq4a</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tis’ the damn season!! </t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bkocaonkoo7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1hhdm3z</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Serene green </t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgia2hnono7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1hhda8q</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>Stuck cap help?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hhda8q/stuck_cap_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1hhcuhc</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Comparison requests Cracked Polish and DVN </t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hhcuhc/comparison_requests_cracked_polish_and_dvn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1hhc83w</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails 4 months ago VS natural nails today (15+ year nail biter) </t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhc83w</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1hhbywk</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Looks like it'll be another green winter</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9qau35uao7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1hhbw2y</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Shortoiseshell 🐢</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/unr5vkm8ao7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1hhbg5x</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>Nice velvet results with a magnetic wreath hook</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhbg5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1hhb1h7</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>The hype is real - ILNP flower child 🦄</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhb1h7</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1hhazxx</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Wicked inspired nails</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhazxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1hhazwb</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>Emergency question</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b4ukgcre3o7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1hhagrn</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Cheers to Cozy Season!</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhagrn</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1hha6t1</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Might not exist, but is there a dupe for this?</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hha6t1</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1hha4id</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Nail polish collection</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hha4id/nail_polish_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1hha2h4</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>bday nails from the other day</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0dxzv94wn7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1hh9i11</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Gilded</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7j2v17avrn7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1hh8xav</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Arcana is magic </t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uz75shgfnn7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1hh8sv0</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Anyone know of similar polishes? Or will this come back into stock? 🥲</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3tnsr1okmn7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1hh8hy8</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Essie Expressie - Sk8 with destiny</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh8hy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1hh8ht3</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Essie Expressie - Sk8 with destiny</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh8ht3</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1hh84d2</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>I heard we were sharing our Xmas manis🎄💅</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wi3dd7lchn7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1hh7gh3</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Gift for nail salon?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hh7gh3/gift_for_nail_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1hh7coo</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>I feel like these are lacking something?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7pzrtzhgbn7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1hh71wd</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>Today's Christmassy Nails</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/db2r4ic49n7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1hh6w1m</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Holiday Time! (Is it Skittles if it's 2 colors?)</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mrag9ykn7n7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1hh6q2u</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nails for the week </t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh6q2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1hh6kvp</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>ILNP Dear Santa 😍</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kmh2imgg5n7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1hh6ixt</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>ILNP gift advice please!! for the sake of friendship!!</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hh6ixt/ilnp_gift_advice_please_for_the_sake_of_friendship/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1hh6cok</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has anyone gotten their Zoya BF order yet? </t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hh6cok/has_anyone_gotten_their_zoya_bf_order_yet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1hh66tp</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Berry Moment</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh66tp</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1hh62tj</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Red? For Christmas? Groundbreaking. </t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/je6d8rsn1n7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1hh5w8l</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Brainstorm Polish Gift </t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hh5w8l/brainstorm_polish_gift/</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1hh5r0h</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Shimmer skittle</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/pkybj902zm7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1hh5pmg</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Some BKL BG3 swatches I haven’t seen on here yet </t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh5pmg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1hh5fqy</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Holiday nails</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ejmy9h4owm7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1hh5bqz</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>Forbidden Fruit 🫒🍒</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh5bqz</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1hh4oil</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Kathleen &amp; Co- Return of the Living Dead 2.0 Velvet Style!</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9tb6hewoqm7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1hh4bxd</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>White Christmas ❄️</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh4bxd</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1hh3q7e</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Dupe for BKL - The Black Lion &amp; Silversaint</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hh3q7e/dupe_for_bkl_the_black_lion_silversaint/</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1hh2jwg</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>favorite kbshimmer polishes?</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hh2jwg/favorite_kbshimmer_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1hh26gs</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>✨️🌲Green and Gold🌲✨️</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh26gs</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1hh1isp</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Christmas Hex</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh1isp</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1hh0829</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t xml:space="preserve">what do you think? </t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ueiv0k3xll7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1hh03ul</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>I’m still stuck on a skittle roll. Upcoming:</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b130cqmkkl7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1hgzjvu</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Impulsive ? Who ? Me ? </t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgzjvu</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1hgzi19</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Frosty thermal for winter ❄️ </t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fmaz2ny2dl7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1hgyyyb</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Snail Works Metal Coat</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8adnbwe56l7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1hgydge</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>Tried to do something fancy with my nails for the first time! Mildly pleased with the result.</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6nhz38txk7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1hgovu0</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lurid lacquer </t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgovu0</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1hhltwu</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Van Gogh Starry Night</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gmhzbgperq7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1hhj44x</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>Had a little fun at home and decorated Christmas nails for my cousin &amp; her daughter</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhj44x</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1hhj2je</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ready for Christmas! </t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhj2je</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1hhhu62</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Took several ideas from pinterest and did my best 🤶✨️</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwadc2rxnp7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1hhg9gu</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>For my favourite sub❤️❤️</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhg9gu</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1hhep2e</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Emerald and Gold Nails</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhep2e</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1hheha1</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nails i did for someone </t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlh8gqiquo7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1hhbzi9</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>2 months</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x90gumbzao7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1hhb7b7</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>QUESTION! Gel polish wont cure on nail stand.</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hhb7b7/question_gel_polish_wont_cure_on_nail_stand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1hh9kqj</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Sia Everyday is Christmas album art! I'm so proud if her!</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh9kqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1hh8nvq</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Is everybody’s nail ready for Christmas?😆🎄🎅🏻</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh8nvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1hh7l2m</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Karina_nails_Rodriguez</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44io1dy6dn7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1hh6zpv</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried cat eye </t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh6zpv</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1hh6pkr</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>What do you think of this design chosen by a young girl?</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t1w56eai6n7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1hh5jxg</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>Corpse Bride Press On Nails</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s4fgh6elxm7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1hh4rgm</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>some of my works. which one do you like the most?</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh4rgm</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1hh2dnd</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time! </t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nq4ppf717m7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1hh1rcf</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Christmas set 💅</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh1rcf</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1hh0x5u</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>Striping tape: light color over dark</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hh0x5u/striping_tape_light_color_over_dark/</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1hh0fp3</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>some of my nails</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh0fp3</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1hgzvbc</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Pink holo Xmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hgzvbc</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1hgxnl6</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>Did my own nails 🥹</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k2nfa34onk7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Dec 20 08:10:57 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_22.xlsx
+++ b/data/collected_data/2024_12_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C872"/>
+  <dimension ref="A1:C1059"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15257,6 +15257,3185 @@
         </is>
       </c>
     </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1hif6eo</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>Got bored so did Christmas nails</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2i41m4vnoy7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1hif4jg</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Christmas nails done by me</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hif4jg</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1hies1z</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>I love french ombre 🤍</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hies1z</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1hieg5w</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>pinky set 🎀</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a1kj5civey7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1hieb3c</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday nails </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a9mk8ct2dy7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1hie5r8</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Adore the rainbow flecks &lt;3</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hie5r8</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1hidmcy</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Gift idea for my sister</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hidmcy/gift_idea_for_my_sister/</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1hidipl</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Shien nail drill </t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hidipl/shien_nail_drill/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1hid8c4</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Merry Christannukah, y’all!</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4umot0na0y7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1hid3zr</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>I am obsessed! :)</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c0s162vwyx7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1hicye2</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Christmas yay</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgz5rt45xx7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1hicf0h</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter Snowflake Cat Eye </t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekixdmb7rx7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1hicetp</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ok Nail Crew,  I need your opinion </t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qa781ti5rx7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1hiceo1</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>Can you tell that this is supposed to be a Christmas tree?</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiceo1</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1hic6bz</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder Gel update </t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6jxq3bqoox7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1hic486</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>My bffs attempt at Christmas nails 🎄🐻‍❄️</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hic486</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1hibxqs</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>In loveee</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4py5na07mx7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1hi900p</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gel nails diy! </t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hi900p/gel_nails_diy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1hi9s40</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>nails not fully drying</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rj7fblfd0x7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1hia4pw</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hia4pw</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1hiaqg9</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>How Nails Helped Me Embrace My Disabilities</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiaqg9</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1hiazao</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Any one have suggestions for a birthday set but my birthday is also New Year’s Day.</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hiazao/any_one_have_suggestions_for_a_birthday_set_but/</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1hiawqi</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>I hope you like this simple design 💙</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiawqi</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1hiav3z</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>Icy Nails</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/25hgflk8bx7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1hiaqs1</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Current set🤍</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiaqs1</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1hiapv9</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Crack in Finger</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2tx623q9x7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1hi9tph</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>Slay or nay?</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rigbe65t0x7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1hi9s9i</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>I'll have a blue Christmas....</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi9s9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1hi9l5p</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Hand-painted holiday nails</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi9l5p</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1hi9erg</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>I’m just an elder emo who also wanted a snowflake on my fingers. 🖤❄️</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/417e5ghqww7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1hi9bh9</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new dip mani from @thenailshoplex </t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8aqp55jtvw7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1hi8rba</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Holiday Nails!</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi8rba</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1hi8bie</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just wanted to show off my Christmas nails </t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7k0koescmw7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1hi7m56</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The girl with one arm. </t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi7m56</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1hi811v</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Does anyone know of a gel nail polish that looks similar to this color?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi811v</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1hi7zpp</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>It’s Christmas nail season babyyy</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2cxtlmejw7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1hi7y45</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Crystal glitter nails! 😊</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ujw6qrtyiw7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1hi6qrg</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bloody cuticles? Is this normal? </t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi6qrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1hi7101</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I wanted something not Christmas. </t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1tlcje2raw7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1hi6fx6</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nl581q7n5w7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1hi6d9i</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>Just got ny acrylics off. Is this normal?</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xl6gx7lz4w7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1hi5d9d</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>My first try with rubber base</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hqy9xtvdwv7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1hi58vh</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Pink cat eye nails😍</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g56hfuwdvv7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1hi57r7</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Different Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hi57r7/different_christmas_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1hi2xnv</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>what do i do 😰</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3cg4iy72dv7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1hi45n4</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>Does anyone know how to get this nail polish?</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hi45n4/does_anyone_know_how_to_get_this_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1hi54ol</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>Little reindeer 🦌💜</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi54ol</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1hi54jl</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>I tried the snowflake trend!❄️</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hjvxcaduv7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1hi4f4q</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Time for a new set?</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi4f4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1hi3zy8</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t xml:space="preserve">With a lot of love I show you my nails </t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi3zy8</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1hi3yia</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>Last queen of the day, lover of design and color</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi3yia</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1hi3vvq</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Managed to squeeze in a set of Christmas nails before my wedding nails in a few days!</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sun7e7afkv7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1hi3qsq</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Christmas Mani 🎄</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6ml3gebjv7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1hi3lig</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Addicted to the bright happy colors!</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6nh6q144iv7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1hi33he</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Beautiful pink hand nails to match my toenails</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uiy3oqa3ev7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1hi2jgt</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What service to grow my natural nails </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnvw9unx9v7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1hi2da0</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Christmas set is done!</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi2da0</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1hi23u8</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In love with this colour 😍 </t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w444ffcg6v7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1hi1ys3</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Christmas nails, love them 🎄</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi1ys3</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1hi1ye9</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New New </t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8s971g195v7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1hi1t3q</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>From Mummy to Santa</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5gn3f6t24v7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1hi1dxh</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails ❤️💚🤍 </t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jre86op0v7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1hi1c18</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>Not too bad for press ons!</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bjyb3ga0v7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1hi1bio</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Red Chrome</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s8o8o3220v7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1hi18k0</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Are my nails damaged?</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi18k0</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1hi0y0n</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>I just broke one of my natural nails that’s I’ve been growing out for 6 months😭😭😭😭help!!! What do I do???</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6zt77287xu7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1hi0z16</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>my take on holiday nails</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fguoor5fxu7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1hi0xhw</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>What nail shape should I go for?</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi0xhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1hi0x6w</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Red nails are the best for the winter ❄️❗️</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi0x6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1hi0v5e</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t xml:space="preserve">XXL christmas! </t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ke5829zjwu7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1hi0sgu</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>What do y’all think of my nails??? Xmas edition</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi0sgu</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1hi0mr0</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>In my green era 💚🍀🎄🌿🦎👒</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pi1vj41ruu7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1hi0gjp</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Had so much fun doing holiday sets for friends/family 💚❤️</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi0gjp</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1hi03mq</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>penultimate job of the day 💍</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8evo7n3oqu7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1hhzhda</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Winter nails ❄️</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uvjka65zlu7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1hhzft0</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Chip shop vs nail tech</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhzft0</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1hhz158</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>My nailtech girlfriend is getting depressed because she takes too long to finish procedure</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hhz158/my_nailtech_girlfriend_is_getting_depressed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1hhz0qe</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>Gingerbread Nails! (Done by @Divabeauty_nailspa on Instagram)!</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhz0qe</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1hhz34m</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>✨️🌙💛</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhz34m</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1hhyzuu</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t xml:space="preserve">pov: i like my nails messy </t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7k38z897iu7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1hhyy05</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Christmas!!!! Really proud of these 🤗</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4y81h8vhu7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1hhyqn9</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t xml:space="preserve">builder gel + coffin gel tips :3 sailor moon charms </t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhyqn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1hhypo9</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Weak natural nails from press on</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hhypo9/weak_natural_nails_from_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1hhynax</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How much would you pay for this gel x set? </t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhynax</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1hhyj72</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Black marble 🖤</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c8n4deeteu7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1hhyhms</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>my new nail tech understood the assignment 🌿</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/15djuzeieu7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1hhxxz0</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Winter nails</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vdzxq8b9au7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1hhxuq4</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Double French tips ♥️❤️</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rl39eghl9u7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1hhxrd9</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I am in love </t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhxrd9</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1hhxjpo</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>Nail Wraps, credit to ClebleNails on Etsy</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gf5mqp797u7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1hhxjkd</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>My last two sets, I love my nail tech! 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhxjkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1hhx3jz</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Frosty pink vibes 💖</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhx3jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1hhx15s</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>my new set 💅🏼 thoughts?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5bu885xa3u7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1hhtojm</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Nail art with dip nails, is it possible?</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hhtojm/nail_art_with_dip_nails_is_it_possible/</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1hhvawp</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Not Sure How to Title This??</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hhvawp/not_sure_how_to_title_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1hhvvw1</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Cuticles cut and bled, scared of infection</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hhvvw1/cuticles_cut_and_bled_scared_of_infection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1hhqk0l</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Painted my xmas nails myself</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhqk0l</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1hhr6mb</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>My first red set!</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8egf2g2rms7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1hhtoum</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Kiara sky gel polish darkened after only 7 days?</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhtoum</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1hhwaf7</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>New nails ❤️❤️</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zw65kujxt7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1hif09r</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best Peel Off Base Coat? </t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s7i9av0fmy7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1hievsc</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Random xmas vibes</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hievsc</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1hidxvw</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Improving Slowly But Surely </t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hidxvw</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1hidkon</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Okay, I get it now</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hidkon</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1hiczbw</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Ignore the flooded cuticles, but my new favorite: Chiffon'd of you by OPI.</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4zdmlkkfxx7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1hickse</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>My collection!</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hickse</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1hic7l5</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>Ugh - just did this mani two days ago, took off a band-aid today and ended up with this 😭</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzv7acy1px7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1hic7a8</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Pearly Whites</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hic7a8</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1hiat52</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>I’m so proud of this</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiat52</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1hiapny</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Broken nail, but make it cute 💝</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiapny</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1hi9rym</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>Fool's gold is my new everything</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi9rym</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1hi9o48</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Haven't been feeling red and green this season, so I decided to pay homage to "a major award" instead</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi9o48</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1hi9jlu</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Do any of you remember this stuff?!</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi9jlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1hi9fab</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Christmas magic ✨</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi9fab</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1hi9cuf</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Peppermint Vibes for Christmas</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi9cuf</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1hi982k</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Who's shipping nail lovelies quickly?</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hi982k/whos_shipping_nail_lovelies_quickly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1hi8s0p</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Got the blues</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sql5f01nqw7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1hi88oh</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Question about CVS Essie loyalty program </t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hi88oh/question_about_cvs_essie_loyalty_program/</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1hi7so3</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>Looking for a hot pink magnetic polish (not gel!)</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi7so3</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1hi7hxs</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>First Solar Polish!</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi7hxs</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1hi77f6</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Getting the hang of velvets!</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/nkluoow9cw7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1hi70pb</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Help with crisp lines</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r869lfpoaw7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1hi6n5s</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> CHRISTMAS NAIL STICKERS!!!! </t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi6n5s</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1hi5ur9</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>The most extra colour</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/bm3ngs9h0w7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1hi5neb</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>Had my nails bare for a few hours….</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi5neb</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1hi5m6f</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>2nd attempt at gel polish on myself :)</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi5m6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1hi5j23</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t xml:space="preserve">"I surely have nothing quite like this in my polish collection..." </t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dxdlnazoxv7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1hi57es</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>KBShimmer crushing it</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxxso3x1vv7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1hi4sjc</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Zoya haul from Black Friday</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi4sjc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1hi4isw</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love how this looks in different lighting scenarios </t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfz6i8mipv7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1hi40w6</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>Skittle - Oops all purple!</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi40w6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1hi3o77</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Party Punch in the afternoon sun is chef’s kiss 💋 </t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/31o26i9riv7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1hi3lgi</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>Fields of Lavender Swatches</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6s9uopy5iv7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1hi3bn9</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Ethereal - Witch Of The Waste</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi3bn9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1hi35wv</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Falling snow on a dark night</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi35wv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1hi315y</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>'Cuz I need a little Christmas... right this very minute</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7p12q8qdv7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1hi2o5z</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Tried a gradient</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi2o5z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1hi1srg</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My mini Bees Knees Lacquer haul🐝💅🏾 </t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi1srg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1hi1i5d</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why can't I get my stamp to transfer all the way to the cuticle? </t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi1i5d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1hi17pm</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Did I get scammed?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hi17pm/did_i_get_scammed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1hi12ki</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Don't sleep on L.A. Colors!😍</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi12ki</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1hi10eh</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Experience with AHA nail oils?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hi10eh/experience_with_aha_nail_oils/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1hi0q8s</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Green eyed monster </t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi0q8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1hi0eua</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Most layers of polish you've used in a mani?</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hi0eua/most_layers_of_polish_youve_used_in_a_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1hhzfsl</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>Stunning red and green</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hhzfsl/stunning_red_and_green/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1hhzc80</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>quick dry top coat recommendations?</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hhzc80/quick_dry_top_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1hhywxi</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>Has anyone gotten their order from the BF Zoya sale?</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8dy3xmfohu7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1hhylq4</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Silver and gold ✨</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhylq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1hhxt9z</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your daily nail care essentials? </t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhxt9z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1hhxt5l</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Proud and happily surprised that my regular nail polish mani has lasted me 2 whole weeks!</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhxt5l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1hhxmjo</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Obsessed with Mermaid Bait from MoonCat</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhxmjo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1hhxjyv</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>Ella+mila founder's disappointing views</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hhxjyv/ellamila_founders_disappointing_views/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1hhx91q</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Overdrive Vs Cock A Doodle Doom</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hhx91q/overdrive_vs_cock_a_doodle_doom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1hhx2p4</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Frosty Pink Vibes 💖</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhx2p4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1hhwpyp</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Cirque - Tahitian Pearl</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/phgzt08w0u7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1hhwlfq</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Looking for Habit in nyc/brooklyn! </t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hhwlfq/looking_for_habit_in_nycbrooklyn/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1hhw4xf</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque - Black Swan velvetised </t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhw4xf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1hhvmud</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Blessed with some rare Irish sunshine </t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/miql37b9st7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1hhuybb</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>What happens to returned polish? (Mooncat)</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hhuybb/what_happens_to_returned_polish_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1hhuvyn</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Newbie Laquerista! </t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ycys9yw9mt7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1hhueuh</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>My first nude polish in a long time and I’m in love! I just wish you could see the holo better on camera (second photo is my attempt to show it) - ILNP Bare</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhueuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1hhu75f</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Color in the bottle vs. On the nails </t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dk8juz4fgt7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1hhu677</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My 9 year old said I had to do a “happy holiday” skittle. </t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhu677</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1hhty7b</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Christmas Skittle</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhty7b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1hhtxe3</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can somebody recommend nail lacquer brands that are high quality? </t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hhtxe3/can_somebody_recommend_nail_lacquer_brands_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1hhtsxv</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Sparkle ✨</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhtsxv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1hhtr3o</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help with which nail shapelooks best ? </t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhtr3o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1hhtmth</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Told the Northern lights to keep shining 🌌</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhtmth</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1hhtkbt</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday Nails </t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhtkbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1hh9kt9</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>OPI Chocolate Moose</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hh9kt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1hhsdzc</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>red on short nails is my fave for the holidays!</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvx8aaguzs7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1hhrqpr</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Has this ever happened to you before? </t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhrqpr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1hidilw</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Arcane Jinx inspired Nail Art that I created!</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/icmoa82k3y7e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1hicsi8</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Disappearing snowflakes for a non traditional winter mani.</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hzuh0p0avx7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1hi9mh1</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hand-painted holiday nails </t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi9mh1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1hi9eoj</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I finally got around to doing an arcane set and I love them. The shimmer vial is a liquid nail to add a little more fun. </t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yl5154voww7e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1hi80is</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Sculptural Christmas nude😍</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kmcmw7mjw7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1hi6nxr</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas Blue Set </t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38sqh9an7w7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1hi5zuq</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>had my nails done by my friend, shes really good!</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi5zuq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1hi5q7q</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>A Glam Christmas set🩷 (hand sculpted the present and mug)</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi5q7q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1hi521e</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Nail charms/jewels</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi521e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1hi0ky8</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t xml:space="preserve">White, Champagne &amp; Gold Glow Christmas Set </t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hi0ky8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1hhvqhg</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>Sparkling Christmas Nails ✨</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hhvqhg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1hhstxk</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Icy butterfly 🌬️</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5dgv89f54t7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1hhskjt</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They like? </t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6t2xxhgm1t7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1hhpqg8</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>I don't use gel polish. But I want to create 3d sculpting nail art</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1hhpqg8/i_dont_use_gel_polish_but_i_want_to_create_3d/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1hgkw5g</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>Snowflake</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wws6bxk55h7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Dec 21 08:09:19 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_22.xlsx
+++ b/data/collected_data/2024_12_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1059"/>
+  <dimension ref="A1:C1252"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18436,6 +18436,3287 @@
         </is>
       </c>
     </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1hj34c0</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>My nails vs what I wanted (from the glossychic on Pinterest)</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj34c0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1hj3huw</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Thoughts...?</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrykgpjx458e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1hj337t</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>My first press on set!</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj337t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1hj2s3b</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>My nail tech don’t miss</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj2s3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1hj2kpo</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>Just got my nails done and noticed there are these small dot bubbles surfacing from underneath. How come this happens ?</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ejxedzmu48e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1hj1f74</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Swipe to see the inspo :)) done by me </t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj1f74</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1hj1ks6</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>best press on glues??</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hj1ks6/best_press_on_glues/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1hj1n73</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails! </t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj1n73</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1hj1d6g</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Backed out of Xmas nails last minute but still wanted white, gold, and red. My nail tech did good 🤩</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oetca3och48e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1hj195g</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Some eclectic designs my best friend did this year 🌀🍊🪼</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj195g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1hj0xs7</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Frosty cat eye/monochrome french</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj0xs7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1hj0xby</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Shaping question</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5wy6rlrqc48e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1hj0izd</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Deep red holiday nails</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n4fbvwkp848e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1hj0iz7</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Best nail glue</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hj0iz7/best_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1hj0gml</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>Dip nails clear coat is chipping after for days - is this normal?</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj0gml</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1hj0f01</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Festive </t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zg4b92um748e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1hj03hz</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>Nude Winter Nails ❄️</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kvmvphc448e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1hizwb8</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Red is always the right color</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nm4cyg6a248e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1hizl91</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Subtle Christmas </t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/02jy2wdaz38e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1hix2nd</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I go about buying my girlfriend a nail or salon day? </t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hix2nd/how_do_i_go_about_buying_my_girlfriend_a_nail_or/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1hix59x</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Goth inspired nails </t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hix59x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1hiyosd</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>fresh christmasy nails inspired by cynthia eviro</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiyosd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1hixwhc</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>is it normal for my nails to look like this under my acrylic? is this a fungus?</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hixwhc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1hiz1ej</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>My Nail Tech Kills It</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiz1ej</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1hiz028</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t xml:space="preserve">🍷🎄 </t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcjrunket38e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1hiyna3</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Encapsulated nails designs</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiyna3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1hiy6cg</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A witchy Christmas moment </t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hiy6cg/a_witchy_christmas_moment/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1hixv8s</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fixed my choppy nails with just these two things </t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hixv8s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1hixoyf</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple cow print french tips on my natural nails 🐄🎀🙂‍↔️ </t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hixoyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1hixft3</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Black nails I loved them!</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8qc6qgse38e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1hix5z6</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>Something new for me and at the same time a beautiful happy client 🙈💖</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hix5z6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1hiwwb6</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>🎄 ILNP Holiday Skittle ☃️ Fir Coat 🌲, Say Love ❤️, Empire ✨, and Snow Angel ❄️</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiwwb6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1hiwoci</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So pink and cute! </t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ojfa3ev1838e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1hiwlhx</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>Santa &amp; Helpers</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4fhrkfvb738e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1hiwguy</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mixing glitter in my dip powder is my favorite thing right now. </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pgnc81y6638e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1hiw9c6</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>Here’s one ❄️</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xk6hheae438e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1hiw7a8</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>My holiday nails❤️💚 supposed to be christmas trees. a little grown out, I did them a week ago.</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiw7a8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1hiw6gd</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Festive nails </t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiw6gd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1hivu1s</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cherry nails </t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lr2vjqlr038e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1hivosl</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My penguin nails for Christmas 🎅🏻 </t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hivosl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1hiv6ad</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I tripping? Or do I need to GO BACK? </t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiv6ad</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1hiv2hb</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxrsidv4u28e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1hiuzp7</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Is this normal?</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiuzp7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1hiuwnu</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>(12 Colors of) Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiuwnu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1hius6p</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel Polish Always Peeling off </t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hius6p/gel_polish_always_peeling_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1hiui05</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my own nails! </t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rn7tkf1dp28e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1hiuc63</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just wanted to share my Christmas nails!  </t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a3xm7281o28e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1hiu1ch</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday Nails </t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uyjl0diil28e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1hitts6</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Last set of the year!</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5zl2hwdsj28e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1hitlfy</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>❣️🎄</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n7sg0cfvh28e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1hitkxn</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>E-File (Nail drill) making weird sounds</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5c7psjwqh28e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1hitbmi</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">please help with nail glue on fingers/acrylics!! and also what these should be priced as (for future reference) </t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hitbmi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1hithzv</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Dip + Gel Winter Set</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rii89s2h28e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1hitcj2</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>Holiday festive</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hitcj2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1hisrb8</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Glassy cat eye polish is my new obsession</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9533yh20b28e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1his2fs</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>1930’s nails inspo</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38r03jog528e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1hirx5d</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing my own gel at home. Definitely need to improve but not as bad as I thought I was going to be. </t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1v4ciob428e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1his5h6</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Just in time for Christmas ❄️</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1his5h6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1his4hi</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Christmas nails 🎄</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1his4hi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1his0dr</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Christmas set ❤️</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/buh08574528e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1hir2rp</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Christmas Set 🎄</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uv5vxohjx18e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1hirj5u</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hirj5u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1hiriwz</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Bit of a weird one... favourite brand washing up gloves?</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hiriwz/bit_of_a_weird_one_favourite_brand_washing_up/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1hircj5</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kinda obsessed 😍 </t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdicmpjpz18e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1hir6bf</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>wedding nails</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/plmgfesby18e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1hir4ll</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>Too thick?</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hir4ll</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1hir09i</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">white xmas nails ❄️ ☃️ </t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hir09i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1hiqvy1</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>I´m in love</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g17jsw4xv18e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1hiqpqx</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>I am Smitten with my Barbie Christmas 🎄 Nails 💅🏻 ❄️🩷</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiqpqx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1hiqoai</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Did my own nails</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i12sgruau18e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1hiqbxi</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying this again </t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiqbxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1hiq9zj</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>How do I do a pedicure on myself without breaking my back and hating every second 😅</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hiq9zj/how_do_i_do_a_pedicure_on_myself_without_breaking/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1hipzy6</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A friendly reminder to use HEMA free gel polish </t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hipzy6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1hipsvh</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>First time using polygel</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hipsvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1hipn6k</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>Peachy French Tips</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hipn6k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1hip2z3</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t xml:space="preserve">long time lurker first time poster </t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hip2z3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1hiolav</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>Christmas set! In Love</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiolav</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1hioi5q</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Are these supposed to be reusable?</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1pgz2lwad18e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1hiohni</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Have never had acrylic nails before but love them even if Kevin is bored of them.</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a16sqr35d18e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1hiobpk</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Silver Bells</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2boiopvxb18e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1hio8yi</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hio8yi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1hie12n</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>How do I get my soft gel tips to stay on longer?</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hie12n/how_do_i_get_my_soft_gel_tips_to_stay_on_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1hij2l4</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hij2l4/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1hijsw6</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Trying Builder Gel - Questions </t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/up1annct908e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1hilg3q</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Little Christmas boy </t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hilg3q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1hiljlx</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>What is this shape called?</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7f2xdl5dp08e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1hinl02</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bio gel &amp; opi gel </t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hinl02/bio_gel_opi_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1hins2h</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>Longest Lasting DIY? Gel, Dip, etc?</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hins2h/longest_lasting_diy_gel_dip_etc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1hinq65</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Can’t decide if my new nails give off an icy or a mermaid vibe</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hinq65</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1hinq4t</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>All-out Christmas builder gel 🎄❄️✨️🎁</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hinq4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1hinou0</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>White &amp; golden</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7be90jry618e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1hinlgi</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it possible to apply handmade press-on nails with the same method as acrylic nail tips? </t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hinlgi/is_it_possible_to_apply_handmade_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1hin5rl</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Spooky gingerbread set👻🎄</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2388o3q218e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1himeuh</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Sharing some of my recent work 💗😊</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1himeuh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1hilk3j</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails </t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hilk3j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1hilgjo</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vortex by W7 </t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hilgjo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1hilanc</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cut my nails short and decided to compensate with the most detailed nail art I’ve ever attempted. </t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hilanc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1hiklhr</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t xml:space="preserve">glitter rainfall, with a dark frenchie </t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pdmbhah7h08e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1hik5d2</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>I need some help!!!</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gx06s5u5d08e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1hiiz73</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Simple set for the holiday season ✨🌌</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiiz73</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1hj4p33</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Obsessed with my Christmas nails 😍</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xivqcr1zj58e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1hj4ovd</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>Vote for ur fave! ✨️</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj4ovd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1hj3yb2</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Glitzy (if only my nails were long…) </t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj3yb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1hj3um8</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>Christmas mani 🎄</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w4gv9d77958e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1hj3i77</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Looking for Chunky Glitters in Jelly</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj3i77</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1hj31xm</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Xmas mooncat</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4k7gzc1wz48e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1hj2d0o</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t xml:space="preserve">‘tis the season </t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj2d0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1hj1ttd</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Cirque colors CS</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hj1ttd/cirque_colors_cs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1hj10ed</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>Mooncat Moonjelly</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj10ed</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1hj0n4p</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>My take on holiday nails</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/flpq7tyv948e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1hj0jk4</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is formulaprofi legit? </t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hj0jk4/is_formulaprofi_legit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1hj0jb5</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t xml:space="preserve">EDM Current Events appreciation </t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj0jb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1hj0402</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Floral Christmas 🌹 </t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj0402</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1hj015z</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Trying out a jelly sandwich. Look okay? Starrily plus Fancy gloss</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj015z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1hizypy</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>Nails peeling at the top?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hizypy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1hiz8ir</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First foray with reflective glitter! </t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiz8ir</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1hiz8fk</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiz8fk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1hiz8f0</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>🤔🤔🤔 The Ethereal/Lumen faux monopoly grows I guess?</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2if7cnaov38e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1hiz4xv</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Reflective glitter = 2025 trend</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hiz4xv/reflective_glitter_2025_trend/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1hiz4or</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter Sparkle Skittle ❄️ </t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiz4or</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1hiysmc</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sparkles for the holiday ✨ </t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p5oaz1ver38e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1hiyb9n</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>99% sure I just ruined the bottle, but does anyone know if this is fixable?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiyb9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1hixy98</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Where to buy polish storage locally?</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ocos3s9ij38e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1hixqi1</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Swatching/organizing my collection </t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hixqi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1hixqd7</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Has anyone ever had this happen with KBshimmer?</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hixqd7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1hixifk</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>I’m a little confused by what happened here, this doesn’t look like the advertised photos at all :(</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hixifk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1hiwwuu</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fresh Mani in Fresh Snow ❄️ </t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiwwuu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1hiwvmb</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t xml:space="preserve">have you ever tried the sally hansen ‘fingerpaints’ line? what did you think of it? </t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiwvmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1hiwumf</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>🎄 ILNP Holiday Skittle ☃️ Fir Coat 🌲, Say Love ❤️, Empire ✨, and Snow Angel ❄️</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiwumf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1hiwpcs</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t xml:space="preserve">LA Colors Mermaid </t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiwpcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1hiw759</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>LynB Designs Cozen</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hiw759/lynb_designs_cozen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1hivx7r</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Christmas lights ✨</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hivx7r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1hivv2m</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>how long does OPI polish typically last paired with essie base coat and essie gel couture top coat?</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hivv2m/how_long_does_opi_polish_typically_last_paired/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1hiva6p</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Endless Blue, gel option</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hiva6p/endless_blue_gel_option/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1hiuszy</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>December nails</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiuszy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1hiuntb</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Nail polish thinner</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hiuntb/nail_polish_thinner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1hiubqy</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Christmas nails! 🎄Mooncat Pandemonium and Serpents of Eden with Holo Taco Scattered Holo Taco</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lns0araxn28e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1hiu4hw</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>thermals are showing me circulation issues i haven’t noticed before 😂</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ypxz4s07m28e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1hip4d2</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Indomitable by Lurid Lacquer 💜</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vsjgy4x4i18e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1hisjyq</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t xml:space="preserve">They're finally free of the strike 😭😭😭 </t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hisjyq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1his1aw</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Cirque Bonbon Jelly</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1his1aw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1hirwyi</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Monarch Ancient Instincts </t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hirwyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1hirrfy</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Favorite Bright Pink Polish?</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hirrfy/favorite_bright_pink_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1hirgr7</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>Hi it is my first time using cat eye nail polish and I like it ♥️</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hirgr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1hirbsm</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>New favorite red ❤️🥰</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hirbsm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1hiqr1d</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Cracked Polish Recommendations?</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hiqr1d/cracked_polish_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1hiqpj8</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Oil spill nails 🌈 </t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/lb1bxlyju18e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1hiqldi</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>Brands with scattered/subtle holo like a-England?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j7fk5ukot18e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1hiqgdy</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dear Santa 🎅 matte and glossy </t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiqgdy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1hiq9wv</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Week 3 of not biting my nails! This is ILNP Chitchat</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ma5crk54r18e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1hiq40j</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>✨️🩰Ballet Slippers🩰✨️</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiq40j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1hiq1yu</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sassy Sauce 5 star customer service </t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hiq1yu/sassy_sauce_5_star_customer_service/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1hiq1yo</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas or the Bulgarian, Hungarian, or Italian flag? You decide. 🇧🇬🇭🇺🇮🇹🎄🎅? </t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiq1yo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1hipwuk</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first non-topper ILNP polish! </t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hipwuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1hipeb4</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Mooncat #1: Maelstrom (or, in my head, Nailstrom)</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hipeb4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1hipcqb</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Chaos skittle of bf buys</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hipcqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1hip640</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>New collab: Orly x Lisa Frank - Thoughts?</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cebw1ocii18e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1hip2u6</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Fields of Lavender 🪻</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2zcakassh18e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1hinunm</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>This past weeks nails 💚</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hinunm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1hincpg</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>Trying to summon some holiday cheer~</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7cshirj9418e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1hinanl</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>Mooncat Out of Stock likelihood for newest rollout?</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hinanl/mooncat_out_of_stock_likelihood_for_newest_rollout/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1himbhw</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>Some holiday manis 🎄</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1himbhw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1him5az</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>No holo for me</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1him5az/no_holo_for_me/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1hill2c</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I *need* a dupe for this </t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3gsm8hypp08e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1hilgyk</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Vortex By W7 </t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hilgyk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1hildrk</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Another Christmas mani</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hildrk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1hikaef</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mery Chrysler ! </t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hikaef</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1hijhid</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>A swirly Christmas 💙❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hijhid</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1hi096k</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Finding nail rings/prosthetic help</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hi096k/finding_nail_ringsprosthetic_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1hi8la6</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice on putting builder gel on overfiled nail </t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8hiy33twow7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1hij3rp</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Mooncat Mercury in Retrograde</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hij3rp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1hiillk</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>something shimmery with a touch of sparkle [products listed]</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiillk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1hifitf</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Striping tape: light color over dark </t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hifitf/striping_tape_light_color_over_dark/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1hj54my</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Elsa Nail art</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbmlfb0xp58e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1hj3j1x</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>🍒</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj3j1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1hj2nex</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Press-ons I made for my little sister!</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/egwo0h6iv48e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1hj0047</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Wicked nails! 🧹🪄🫧👑</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj0047</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1hixqfx</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Black polka dots on cateye tutotial</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wnxjb7cjh38e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1hiwtq5</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Hope this counts: feeling extra festive for Christmas so I made these:)</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qhidef9b938e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1hiv6y1</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>Red &amp; Gold Foil Nails</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiv6y1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1hiuvgz</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>New to the hobby.</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kp9t7ocis28e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1hiu1nb</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>First attempt at marbling</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/037dad0ll28e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1hitzqw</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Green and Icy Silver</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hitzqw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1hitwzm</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>My mom's Xmas nail art! It's simple but it's her first time doing anything like this 💕</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pq536qcik28e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1hisuua</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>Hello, here I am again! Do you like it? I loved them</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hisuua</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1his4vk</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Little green dress with an icy belt buckle!</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zolcrdy2628e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1hiq9qn</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My Christmas Nails! </t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hiq9qn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1hipy6y</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Not bad for starting this month</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hipy6y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1himnj6</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gift I Did For A Friend </t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jut8bxqmy08e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1hikm53</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Honest advice❤️</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d78719vch08e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1hihxkm</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>My new nails</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hihxkm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1hihvjk</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas time is here 🎶 </t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hihvjk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1hifyna</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>I did my Christmas nails, do you like them?</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dmvf41lqzy7e1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Dec 22 08:09:29 UTC 2024
</commit_message>
<xml_diff>
--- a/data/collected_data/2024_12_22.xlsx
+++ b/data/collected_data/2024_12_22.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1252"/>
+  <dimension ref="A1:C1436"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21717,6 +21717,3134 @@
         </is>
       </c>
     </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1hjssbj</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>my new holidays set,done by my nail tech, first pic is in the sunlight and the second one is with flash</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjssbj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1hjsxp2</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>Christmas sparkle ❤️✨🎄💅</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjsxp2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1hjt8nc</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Strongest press ons?</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hjt8nc/strongest_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1hjstou</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Christmas Nails ☃️🎄</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dm7xclvwec8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1hjsn62</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Losing a finger nail. Ever lost one completely? </t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/as8ir0xkcc8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1hjsmbb</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>Is my manicure putting you in the New Year's mood</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/on25hs25cc8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1hjs8eq</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>First time coloring my nails. It's messy but it was so much fun. My wife agrees!</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjs8eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1hjrzcj</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>Got my nails done today!</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jg7wb3kb4c8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1hjr2d0</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Is it normal for nail tech to use different technique?</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjr2d0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1hjph9v</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Low damage at home options?</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hjph9v/low_damage_at_home_options/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1hjouhn</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>HELP (gelx)</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4n5hh6ag5b8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1hjrk2u</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>my holiday nails</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjrk2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1hjrekh</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2 Month Nail Journey </t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjrekh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1hjrdyt</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>The ugliest French tips I’ve ever seen?</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjrdyt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1hjr1dk</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>✨ Rhinestones✨ for the Holidays! 🎄</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjr1dk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1hjqwlv</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cuticles </t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjqwlv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1hjqw0a</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lovin’ these winter nails </t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/npdogmuqrb8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1hjqd9m</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Birthday Nails</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/woo90cmylb8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1hjpu54</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Last months nails and this months 🖤</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjpu54</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1hjpsti</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>She has been Saved 🙏</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjpsti</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1hjpqgf</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Christmas ready 🎄</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tsibe3a1fb8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1hjnzqs</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple yet I love them! Done by myself :) </t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6qwvyzlwa8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1hjnvxf</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>My DIY✨Christmas✨ nails</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjnvxf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1hjnvj7</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying </t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/af68mt1gva8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1hjnv4z</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Cuticle nipping! HELP!</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hjnv4z/cuticle_nipping_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1hjngug</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Festive set</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kxs5r1gra8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1hjne8n</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>Sparkle blue mani!</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7puyrgbqqa8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1hjn59q</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t xml:space="preserve">obsesseddd with this set! </t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjn59q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1hjn3ph</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Filing dip thinner</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hjn3ph/filing_dip_thinner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1hjmqz5</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Before and after doing a mani pedi on myself </t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjmqz5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1hjmqd7</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Merry Christmas 🎄🎁 </t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/78drz8bfka8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1hjmpbq</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Pink Chrome!</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uj1aolz4ka8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1hjmlx7</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Engagement Nails! </t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgsr2mu9ja8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1hjlxc9</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Junk nails!💖 definitely my favorite set I’ve ever gotten </t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjlxc9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1hjmhp3</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Today . I’m happy </t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kdguis6ia8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1hjly6p</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>First set of acrylics.... How would you rate these?</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjly6p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1hjlqox</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Holiday set ❄️ </t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xjo8m7jzaa8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1hjlofr</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel X, I’ve done my nails yesterday and they are popping off today. Please help </t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hjlofr/gel_x_ive_done_my_nails_yesterday_and_they_are/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1hjlgn7</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>Red</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/48ayrrsf8a8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1hjlfz8</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>Last Christmas set 🎅</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5pivz8x98a8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1hjlcrf</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>My wife (F) has been painting my (M) nails since we got bored during the pandemic. This is the first time I get them professionally done and first time getting gel.</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://giphy.com/gifs/WQq5oce6OPuJF1d7VB</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1hjl74i</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>Holiday nails! What do you think? ❤️💚🎄</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h0s93uh16a8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1hjkq54</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>How long should a manicure/gel nails last?</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjkq54</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1hjkptx</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>New client and she was happy with her design, I hope you like it</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjkptx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1hjkp3m</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1cf0rjcu98e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1hjk11x</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>Deep sienna/umber?</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hjk11x/deep_siennaumber/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1hjk8z3</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Christmas Nails (First Post!)</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjk8z3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1hjkeli</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Not so Christmas “Christmas” nails </t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oh9lro01z98e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1hjk2kn</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>Ready for Christmas!</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xh184fj3w98e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1hjjry1</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter midnight nails </t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/90magk1ht98e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1hjjp24</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>christmas nails i did on myself🎄</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjjp24</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1hjjnog</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">my nails for my holiday trip! I’m so happy with how they came out </t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjjnog</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1hjjmd4</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>My nails keep lifting</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hjjmd4/my_nails_keep_lifting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1hjium2</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>My first time doing French tip nails. How did I do?</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjium2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1hjirrk</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>Peppermint Nails for the Holidays🍬</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvsb81ulk98e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1hjikgh</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need advice on length </t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjikgh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1hjijag</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>What do you think of my nails for Christmas?</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mjuj6b4ji98e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1hjiafs</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>Shaping flared nails</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bto5ijcdg98e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1hji5sx</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>My self-painted nails this year from May to this morning</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hji5sx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1hjhvz8</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>cat eye design 🥰</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/t8me8chqc98e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1hjhqkd</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/961g5o8nb98e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1hjhpgk</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>Christmas ready 🎄</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p4kpvpfdb98e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1hjhgbt</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Happy holiday 1994 - Barbie serie season 1</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjhgbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1hjh11z</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Happy Winter Solstice</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dqw0shh598e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1hjg300</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Simple and Elegant for the Holidays 💕</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87oa3imkx88e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1hjg1o8</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>cat eye design🥰</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/b1utv8b4x88e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1hjfvt8</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Do you like it?</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oj14ho4yv88e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1hjfe4m</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>At first I didn’t like the color. But slowly this “Ice Queen” sparkles are starting to grow on me.</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/epuhogivr88e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1hjfd2s</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cult of the Lamb </t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ueudzubmr88e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1hjf6ev</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>Gingerbread nails i did on myself 💖</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjf6ev</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1hjf3zw</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>New fill yesterday. Im addicted to this style of french tip</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myo3ntnlp88e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1hjf05t</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Suggestions for a nice iridescent (blueish-pink-purplish-white) polish?</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hjf05t/suggestions_for_a_nice_iridescent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1hjevjb</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Festive nails (attempt)</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yr4wds0on88e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1hjegj6</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Festive nails ✨</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxbuadl8k88e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1hjedi1</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Hi - I have short nails and want to try the ombre technique. What advice/tips can you give me?</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1hjedi1/hi_i_have_short_nails_and_want_to_try_the_ombre/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1hje6mn</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Emerald structured French tips</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hje6mn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1hje5ow</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>Christmas nails</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hje5ow</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1hje4o9</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Last nails of the year! Needed something that would fit both Christmas and New Year’s </t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hje4o9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1hjdz0w</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My 1st almond-shaped nails💅 </t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjdz0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1hjdvvc</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ready for the holidays! </t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjdvvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1hj5aqa</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>🦋</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/muw4ggh5s58e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1hjb3wp</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>what i asked for vs. what i got</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjb3wp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1hjca88</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t>Merry Christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y62squ1t188e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1hjcbxy</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>Chanukkah Nails!!</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iw9ledz7288e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1hjdbn8</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Christmas nails 🦌 </t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exg93ocsa88e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1hjczj6</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>my clown nails 🤡</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1wk0kpu788e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1hjcy8c</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>Christmas goldies 💫💅🏼</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35n65jbj788e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1hjcp47</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t>thoughts?</t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j9ukh68g588e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1hjc0o8</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Did not had a good day with doing my nails but they're okay ish, what do you think?☃️❄️💙</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjc0o8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1hjc016</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">December Nails - GelX </t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjc016</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1hjbz1n</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>Can't stop staring at them 👀</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jomtplz2z78e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1hjbpsb</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t>Puede que no sean diseños extravagantes, pero estoy satisfecho y feliz con el trabajo realizado para mis clientes estrella 🙈🥰</t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjbpsb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1hjbp30</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>Loving my Christmas nails 💅🤶🏽✨</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ndql36kw78e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1hjbm5s</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xy30alutv78e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1hjbjww</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Red fixes everything! Now I'm ready for Christmas</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/km9xgu3av78e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1hjbj61</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>New Year’s nails!</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ywbutzc3v78e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1hjbe2w</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t>summer color for Christmas 😭ate tho</t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gqy68e4st78e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1hja83o</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Do you like this style?</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8kij2pii78e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1hj9yop</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t>Shout out to talented nail techs</t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aj0bqltuf78e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1hj9rq5</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>I'm learning to do 3d acrylic flowers. I'm really proud of these two</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://i.imgur.com/xX8Glc7.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1hjsjzz</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t>Reorganizing my polishes</t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjsjzz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1hjrjm6</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t>Looking for a purple and green polish (shimmer, duo/multi-chrome, flakies)</t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hjrjm6/looking_for_a_purple_and_green_polish_shimmer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1hjqm0p</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Looking for a grey base nail polish with purple shimmers</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hjqm0p/looking_for_a_grey_base_nail_polish_with_purple/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1hjqggj</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Snowflake Glitter Accent</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96zqdyyzmb8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1hjqgcs</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t xml:space="preserve">a little Fancy Gloss x Chappell color match </t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjqgcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1hjqexj</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>smell of filing nails</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hjqexj/smell_of_filing_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1hjpgcw</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Lightning McQueen</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hjpgcw/lightning_mcqueen/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1hjpfpj</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Snow inspired - Curiosity’s Prey</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjpfpj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1hjo948</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>my BF haul arrived 2 days ago and i finally swatched all of them ✨</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjo8i0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1hjo685</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>People keep asking whether my nails are fake when I wear this topper 😍</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wo38zucdya8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1hjo3v0</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t>Mercury's Tears is STUNNING 🩵💙💜🩷</t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjo3v0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1hjnr2m</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Victorian Varnish's Fiery Personality </t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5n60fx29ua8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1hjnkcc</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter Nails! </t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/kd8bbttdsa8e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1hjnhb5</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Just a touch of holiday spirit</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjnhb5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1hjnfoa</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>Christmas Nails</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjnfoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1hjmxfs</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t>Red Chrome Powder on Regular Polish</t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjmxfs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1hjmpmn</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t>Christmas Nails!</t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdgp7sh7ka8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1hjmo0q</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Weekend mani before Xmas! 🎄</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d18pns7tja8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1hjme46</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t>Master list of boutique/indie polishes (please add if you can!)</t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hjme46/master_list_of_boutiqueindie_polishes_please_add/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1hjliv0</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>christmas nail art</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjliv0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1hjl1yv</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>Grinch nails!</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aqkm3a7r4a8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1hjkw5b</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>My first tri-thermal 👀💙</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wfrszndc3a8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1hjknag</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>🤩</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjknag</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1hjkacq</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pangea by Mooncat </t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjkacq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1hjjz5y</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Horseshoe magnet </t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/aut8q5q8v98e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1hjjvp4</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Best hand cream to keep in the cold?</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hjjvp4/best_hand_cream_to_keep_in_the_cold/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1hjjgrw</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t>No Mistakes, just Happy Accidents 💖🌊🎨</t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjjgrw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1hjjbib</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>my first holo tacos!!!</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d8dnqeoep98e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1hjis71</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t>Bright cat eye?</t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hjis71/bright_cat_eye/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1hjirzv</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>ISO silky magnetic polish that isn’t gel</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hjirzv/iso_silky_magnetic_polish_that_isnt_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1hjiowz</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t>Suggestions please</t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hjiowz/suggestions_please/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1hjiijw</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>What is going on here?</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjiijw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1hjig9o</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t>🎄Lil' Deb's X-Mas Tree🎄</t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjig9o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1hji7zp</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KBShimmer Berry and Bright. </t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6guq1jxrf98e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1hjhxa9</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>BF Daisychain Polish haul! 🌼 💅</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjhxa9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1hjhpik</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>Polish that got you hooked on indies? (Feat. Cat butt as background)</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vwpxkqjbb98e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1hjhmtq</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Is nail polish supposed to be soft after 24 hours?</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hjhmtq/is_nail_polish_supposed_to_be_soft_after_24_hours/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1hjhben</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t>Rogue Lacquer Black Friday Sale Question</t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i1m1fidz798e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1hjhaf9</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple Christmas nails Glossy &amp; Matte </t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjhaf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1hjh1so</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any tips for how to use DRK Nails Magic Effect For Magnetic Polishes? </t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hjh1so/any_tips_for_how_to_use_drk_nails_magic_effect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1hjgtmx</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Star Wars nails</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjgtmx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1hjgj97</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Is Sally Hansen Miracle Gel HEMA/di-HEMA free?</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hjgj97/is_sally_hansen_miracle_gel_hemadihema_free/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1hjgc1n</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>“What is that, velvet?!”</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xklfzvtoz88e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1hjfs8h</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Clionadh magnetics - Baeocystin, Norpsilocin, Psilocin</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mo8yzzm0v88e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1hjfqou</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Color me Christmas </t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjfqou</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1hjficq</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t>Two color Christmas mani! Mooncat Access Denied and Bottled Rage</t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjficq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1hjfd9a</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are your nail/nail polish goals for 2025? </t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjfd9a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1hjfaxz</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>My first HHC acquisition, I'm happy!</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjfaxz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1hjf8w5</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Solstice Manicure</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0zqkc0ipq88e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1hjf3er</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>My mani for a recent trip to Joshua tree 🐝 🌝</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjf3er</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1hjezil</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t>Christmas mani ❤️🤍</t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imctq9mko88e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1hjeyhn</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Cock a doodle doom unexpectedly dark</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjeyhn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1hjexr6</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t>Holiday mishmash</t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjexr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1hjehlw</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>Super Shiny Christmas Nails ✨💫</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjehlw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1hjecnc</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>Grinch or Ephelba?</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjecnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1hjebeu</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Happy Holidays, Everyone!</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o4m7tnx1j88e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1hje6t7</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love when a polish surprises me by how beautiful it is irl </t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7wggsdhzh88e1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1hjdsl5</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>How to get the thickness of gel with regular polish?</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hjdsl5/how_to_get_the_thickness_of_gel_with_regular/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1hjdhyv</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t>GITD Christmas Lights</t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjdhyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1hjd6ol</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Starting my at home regular polish journey</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjd6ol</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1hjcdyz</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>This is gonna sound crazy, but…shade recs that match this lobster?</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xh5dordq288e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1hjc4wl</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Obsessed with magnetics 🩵</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12oxz84i088e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1hjblg0</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>I’m dreaming of a velvet Christmas 🎄</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjblg0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1hjbakw</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Crazy as glitters </t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjbakw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1hj9qx8</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>This polish exudes magical girl vibes✨</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj9qx8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1hiwf69</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>has mooncat fixed their bottles?</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hiwf69/has_mooncat_fixed_their_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1hiz3o1</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t>Looking for a color similar to A England's Dragon</t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hiz3o1/looking_for_a_color_similar_to_a_englands_dragon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1hj63du</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t>My concert nails!</t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/0sljy4t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1hj5ukz</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>how to prevent green nail syndrome with press on?</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1hj5ukz/how_to_prevent_green_nail_syndrome_with_press_on/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1hjoqyu</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>I think that for next Christmas I will have to practice the snowflake ❄️ 🫣</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yywlhcwf4b8e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1hjoa4a</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>So I have no idea what I'm doing for my wife.</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d6ehs97kza8e1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1hjo7g9</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>Spent my 30th in Mexico with my favorite set I’ve ever done 🏝️🍊</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjo7g9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1hjm7nt</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>I redid my jinx arcane nails</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjm7nt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1hjloea</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I already shared this set but I finally put them on and took some decent pictures. What y'all think? </t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjloea</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1hjhp7z</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t>Happy holiday 1994 - Barbie serie season 1</t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjhp7z</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1hjhl7v</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t>give your opinion</t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjhl7v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1hjgncn</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t>I'm in school and these are a few of my full sets</t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjgncn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1hjfabd</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>This week ✨</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hjfabd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1hje4qy</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Emerald structured French tips</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hje4qy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1hjcbm7</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Winter nails </t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bub2c9j5288e1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1hj9gob</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t>my christmas nails!</t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj9gob</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1hj8qyv</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>concept art for my set</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj8qyv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1hj7kpw</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Christmas bling</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj7kpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1hj6oyn</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>christmas nails🎄</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hj6oyn</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>